<commit_message>
Question list for DP sub sequence
Question list for DP sub sequence
</commit_message>
<xml_diff>
--- a/Dynamic Programming/DP on Subsequences/Question_List-Java version.xlsx
+++ b/Dynamic Programming/DP on Subsequences/Question_List-Java version.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\DP on Subsequences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CECE052-6C76-42B5-836D-C2EB95601B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43124CAA-DA0B-4C47-B9E0-737C9B7E0AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Question No</t>
   </si>
@@ -45,76 +45,19 @@
     <t>GFG/LC/Coding Ninja</t>
   </si>
   <si>
-    <t>Frog Jump</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
-    <t>https://www.codingninjas.com/codestudio/problems/frog-jump_3621012?leftPanelTab=0</t>
-  </si>
-  <si>
-    <t>DP(Recurrsion+Memonization+Tabulation</t>
-  </si>
-  <si>
-    <t>DP(Recurrsion+Memonization+Tabulation+space optimization)</t>
-  </si>
-  <si>
     <t>CN</t>
   </si>
   <si>
-    <t>GFG</t>
-  </si>
-  <si>
-    <t>LC/CN</t>
-  </si>
-  <si>
-    <t>GFG/CN</t>
-  </si>
-  <si>
-    <t>House Robber II-Circular placement</t>
-  </si>
-  <si>
-    <t>Stickler Thief/Maximum sum of non-adjacent elements/House Robber I</t>
-  </si>
-  <si>
-    <t>DP(Space optimizatio)</t>
-  </si>
-  <si>
-    <t>LC</t>
-  </si>
-  <si>
-    <t>Climbing stars</t>
-  </si>
-  <si>
-    <t>DP(Tabulation+space optimization)</t>
-  </si>
-  <si>
-    <t>LC/CN/GFG</t>
-  </si>
-  <si>
-    <t>Unique Paths</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/unique-paths/description/</t>
-  </si>
-  <si>
-    <t>Unique Paths II</t>
-  </si>
-  <si>
-    <t>Minimum Path Sum</t>
-  </si>
-  <si>
-    <t>Maximum Path Sum in the matrix</t>
-  </si>
-  <si>
-    <t>Minimum Falling Path Sum</t>
-  </si>
-  <si>
-    <t>Chocolate Pickup</t>
-  </si>
-  <si>
-    <t>Recurrssion</t>
+    <t>Subset Sum Equal To K</t>
+  </si>
+  <si>
+    <t>DP(Recurrsion+Memonization+Tabulation+Space optimization)</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/subset-sum-equal-to-k_1550954?leftPanelTab=0</t>
   </si>
 </sst>
 </file>
@@ -153,18 +96,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -179,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -206,13 +143,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -505,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,35 +449,35 @@
     <col min="6" max="6" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="16" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" s="13" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15" t="s">
-        <v>7</v>
+      <c r="F1" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -556,167 +486,62 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="8" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="E3" s="8"/>
+    </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>215</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>70</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:6" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>62</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>63</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>64</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
-        <v>931</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>29</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>

</xml_diff>

<commit_message>
GFG. Count Subset with Sum K
GFG. Count Subset with Sum K
</commit_message>
<xml_diff>
--- a/Dynamic Programming/DP on Subsequences/Question_List-Java version.xlsx
+++ b/Dynamic Programming/DP on Subsequences/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\DP on Subsequences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43124CAA-DA0B-4C47-B9E0-737C9B7E0AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63D3F51-6D99-4711-A98D-EA19CB29E76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Question No</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t>https://www.codingninjas.com/codestudio/problems/subset-sum-equal-to-k_1550954?leftPanelTab=0</t>
+  </si>
+  <si>
+    <t>Counts Subsets with Sum K</t>
+  </si>
+  <si>
+    <t>GFG</t>
+  </si>
+  <si>
+    <t>Partition Equal Subset Sum</t>
+  </si>
+  <si>
+    <t>DP(Recurrsion+Memonization+Tabulation)</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -96,12 +111,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -116,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -153,6 +174,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,167 +494,191 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="E3" s="8"/>
-    </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="D9" s="4"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="4"/>
+    <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
       <c r="B12" s="1"/>
+      <c r="C12" s="8"/>
       <c r="D12" s="4"/>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
       <c r="B13" s="1"/>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="6"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="6"/>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
-      <c r="B20" s="6"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
-      <c r="D23" s="6"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="6"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
       <c r="D26" s="6"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
@@ -638,8 +687,8 @@
       <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
     </row>
@@ -650,9 +699,9 @@
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
+      <c r="A30" s="7"/>
       <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
+      <c r="C30" s="6"/>
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -664,34 +713,40 @@
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
-      <c r="C32" s="6"/>
+      <c r="C32" s="8"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CN. Partitions With Given Difference -->(Memoization, space optimization, tabulation)
CN. Partitions With Given Difference -->(Memoization, space optimization, tabulation)
</commit_message>
<xml_diff>
--- a/Dynamic Programming/DP on Subsequences/Question_List-Java version.xlsx
+++ b/Dynamic Programming/DP on Subsequences/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\DP on Subsequences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63D3F51-6D99-4711-A98D-EA19CB29E76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2A475D-433F-4798-9D31-626489385DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Question No</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>Partitions With Given Difference</t>
+  </si>
+  <si>
+    <t>CN/GFG</t>
   </si>
 </sst>
 </file>
@@ -461,7 +467,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -548,9 +554,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>

</xml_diff>

<commit_message>
GFG. 0-1 Knapsack Problem
GFG. 0-1 Knapsack Problem
</commit_message>
<xml_diff>
--- a/Dynamic Programming/DP on Subsequences/Question_List-Java version.xlsx
+++ b/Dynamic Programming/DP on Subsequences/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\DP on Subsequences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2A475D-433F-4798-9D31-626489385DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76748947-AA04-4690-BB4F-C14468FA7553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Question No</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>CN/GFG</t>
+  </si>
+  <si>
+    <t>GFG/CN</t>
+  </si>
+  <si>
+    <t>0 - 1 Knapsack Problem</t>
   </si>
 </sst>
 </file>
@@ -467,7 +473,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,8 +578,18 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
494. Target Sum -->Tabulation approach
494. Target Sum -->Tabulation approach
</commit_message>
<xml_diff>
--- a/Dynamic Programming/DP on Subsequences/Question_List-Java version.xlsx
+++ b/Dynamic Programming/DP on Subsequences/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\DP on Subsequences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE741F8-D557-4EF5-9AE6-7BE6D011AC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6B90BA-2AD3-4D40-BB42-B6B2928F765C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>Question No</t>
   </si>
@@ -72,9 +72,6 @@
     <t>DP(Recurrsion+Memonization+Tabulation)</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>Partitions With Given Difference</t>
   </si>
   <si>
@@ -91,6 +88,12 @@
   </si>
   <si>
     <t>Coin change</t>
+  </si>
+  <si>
+    <t>Target Sum</t>
+  </si>
+  <si>
+    <t>Tabulation</t>
   </si>
 </sst>
 </file>
@@ -129,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,6 +142,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -155,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -196,6 +205,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +495,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,32 +582,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
+    <row r="5" spans="1:6" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="B5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>4</v>
@@ -605,23 +621,35 @@
         <v>322</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="4"/>
+      <c r="E7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>494</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -632,9 +660,7 @@
     <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8"/>
     </row>

</xml_diff>

<commit_message>
Coding ninja. Unbounded Knapsack
Coding ninja. Unbounded Knapsack
</commit_message>
<xml_diff>
--- a/Dynamic Programming/DP on Subsequences/Question_List-Java version.xlsx
+++ b/Dynamic Programming/DP on Subsequences/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\DP on Subsequences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6B90BA-2AD3-4D40-BB42-B6B2928F765C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C13DE3-9066-4A4A-8EE7-E0137652FE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>Question No</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Tabulation</t>
+  </si>
+  <si>
+    <t>Unbounded Knapsack</t>
   </si>
 </sst>
 </file>
@@ -132,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +154,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -164,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -212,6 +221,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,7 +511,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D12" activeCellId="1" sqref="C12 D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,20 +632,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:6" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19">
         <v>322</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="19" t="s">
         <v>9</v>
       </c>
     </row>
@@ -651,11 +667,22 @@
       </c>
       <c r="F8" s="18"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="8"/>
+    <row r="9" spans="1:6" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>

</xml_diff>

<commit_message>
141. Linked List Cycle
Brute force approach updated
</commit_message>
<xml_diff>
--- a/Dynamic Programming/DP on Subsequences/Question_List-Java version.xlsx
+++ b/Dynamic Programming/DP on Subsequences/Question_List-Java version.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\DP on Subsequences\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\Desktop\GIT\Leetcode\Dynamic Programming\DP on Subsequences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8D2658-5076-42BF-A793-A40DB266BE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878E70F0-34C5-4935-A26E-FBEA5A0FB410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -190,26 +190,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -514,7 +501,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,64 +510,64 @@
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="70.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" customWidth="1"/>
     <col min="6" max="6" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="13" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:6" s="8" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:6" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -597,24 +584,24 @@
       <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -631,67 +618,67 @@
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
+    <row r="7" spans="1:6" s="15" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
         <v>322</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+    <row r="8" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
         <v>494</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="18"/>
-    </row>
-    <row r="9" spans="1:6" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:6" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -700,22 +687,22 @@
       <c r="D10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="8"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
-      <c r="C12" s="8"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="8"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -743,128 +730,99 @@
     </row>
     <row r="18" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="5"/>
+      <c r="B18" s="1"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="5"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
+      <c r="A21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="5"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="6"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="5"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
+      <c r="A27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
+      <c r="A28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
+      <c r="B29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+      <c r="B30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="6"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="6"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
     </row>
   </sheetData>

</xml_diff>